<commit_message>
Adjusts 2020 GDP to match COVID-related output drop
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EGGRA/Exogenous GDP Growth Rate Adjustment.xlsx
+++ b/InputData/ctrl-settings/EGGRA/Exogenous GDP Growth Rate Adjustment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\ctrl-settings\EGGRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCB0B47-18DD-4966-843A-5A57976B2B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C119599B-4CDC-4462-8A1A-3CD2267D0129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="16170" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26640" yWindow="2160" windowWidth="23505" windowHeight="13065" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1204,12 +1204,6 @@
     <xf numFmtId="166" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1220,6 +1214,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1560,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1758,7 +1758,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7387,238 +7387,238 @@
       </c>
     </row>
     <row r="121" spans="1:16" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A121" s="77" t="s">
+      <c r="A121" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="B121" s="78"/>
-      <c r="C121" s="78"/>
-      <c r="D121" s="78"/>
-      <c r="E121" s="78"/>
-      <c r="F121" s="78"/>
-      <c r="G121" s="78"/>
-      <c r="H121" s="78"/>
-      <c r="I121" s="78"/>
-      <c r="J121" s="78"/>
-      <c r="K121" s="78"/>
-      <c r="L121" s="78"/>
-      <c r="M121" s="78"/>
-      <c r="N121" s="78"/>
+      <c r="B121" s="76"/>
+      <c r="C121" s="76"/>
+      <c r="D121" s="76"/>
+      <c r="E121" s="76"/>
+      <c r="F121" s="76"/>
+      <c r="G121" s="76"/>
+      <c r="H121" s="76"/>
+      <c r="I121" s="76"/>
+      <c r="J121" s="76"/>
+      <c r="K121" s="76"/>
+      <c r="L121" s="76"/>
+      <c r="M121" s="76"/>
+      <c r="N121" s="76"/>
     </row>
     <row r="122" spans="1:16" s="69" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="75" t="s">
+      <c r="A122" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="B122" s="75"/>
-      <c r="C122" s="75"/>
-      <c r="D122" s="75"/>
-      <c r="E122" s="75"/>
-      <c r="F122" s="75"/>
-      <c r="G122" s="75"/>
-      <c r="H122" s="75"/>
-      <c r="I122" s="75"/>
-      <c r="J122" s="75"/>
-      <c r="K122" s="75"/>
-      <c r="L122" s="75"/>
-      <c r="M122" s="75"/>
-      <c r="N122" s="75"/>
+      <c r="B122" s="73"/>
+      <c r="C122" s="73"/>
+      <c r="D122" s="73"/>
+      <c r="E122" s="73"/>
+      <c r="F122" s="73"/>
+      <c r="G122" s="73"/>
+      <c r="H122" s="73"/>
+      <c r="I122" s="73"/>
+      <c r="J122" s="73"/>
+      <c r="K122" s="73"/>
+      <c r="L122" s="73"/>
+      <c r="M122" s="73"/>
+      <c r="N122" s="73"/>
     </row>
     <row r="123" spans="1:16" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A123" s="75" t="s">
+      <c r="A123" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="B123" s="76"/>
-      <c r="C123" s="76"/>
-      <c r="D123" s="76"/>
-      <c r="E123" s="76"/>
-      <c r="F123" s="76"/>
-      <c r="G123" s="76"/>
-      <c r="H123" s="76"/>
-      <c r="I123" s="76"/>
-      <c r="J123" s="76"/>
-      <c r="K123" s="76"/>
-      <c r="L123" s="76"/>
-      <c r="M123" s="76"/>
-      <c r="N123" s="76"/>
+      <c r="B123" s="74"/>
+      <c r="C123" s="74"/>
+      <c r="D123" s="74"/>
+      <c r="E123" s="74"/>
+      <c r="F123" s="74"/>
+      <c r="G123" s="74"/>
+      <c r="H123" s="74"/>
+      <c r="I123" s="74"/>
+      <c r="J123" s="74"/>
+      <c r="K123" s="74"/>
+      <c r="L123" s="74"/>
+      <c r="M123" s="74"/>
+      <c r="N123" s="74"/>
     </row>
     <row r="124" spans="1:16" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A124" s="75" t="s">
+      <c r="A124" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="B124" s="76"/>
-      <c r="C124" s="76"/>
-      <c r="D124" s="76"/>
-      <c r="E124" s="76"/>
-      <c r="F124" s="76"/>
-      <c r="G124" s="76"/>
-      <c r="H124" s="76"/>
-      <c r="I124" s="76"/>
-      <c r="J124" s="76"/>
-      <c r="K124" s="76"/>
-      <c r="L124" s="76"/>
-      <c r="M124" s="76"/>
-      <c r="N124" s="76"/>
+      <c r="B124" s="74"/>
+      <c r="C124" s="74"/>
+      <c r="D124" s="74"/>
+      <c r="E124" s="74"/>
+      <c r="F124" s="74"/>
+      <c r="G124" s="74"/>
+      <c r="H124" s="74"/>
+      <c r="I124" s="74"/>
+      <c r="J124" s="74"/>
+      <c r="K124" s="74"/>
+      <c r="L124" s="74"/>
+      <c r="M124" s="74"/>
+      <c r="N124" s="74"/>
     </row>
     <row r="125" spans="1:16" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A125" s="75" t="s">
+      <c r="A125" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="B125" s="76"/>
-      <c r="C125" s="76"/>
-      <c r="D125" s="76"/>
-      <c r="E125" s="76"/>
-      <c r="F125" s="76"/>
-      <c r="G125" s="76"/>
-      <c r="H125" s="76"/>
-      <c r="I125" s="76"/>
-      <c r="J125" s="76"/>
-      <c r="K125" s="76"/>
-      <c r="L125" s="76"/>
-      <c r="M125" s="76"/>
-      <c r="N125" s="76"/>
+      <c r="B125" s="74"/>
+      <c r="C125" s="74"/>
+      <c r="D125" s="74"/>
+      <c r="E125" s="74"/>
+      <c r="F125" s="74"/>
+      <c r="G125" s="74"/>
+      <c r="H125" s="74"/>
+      <c r="I125" s="74"/>
+      <c r="J125" s="74"/>
+      <c r="K125" s="74"/>
+      <c r="L125" s="74"/>
+      <c r="M125" s="74"/>
+      <c r="N125" s="74"/>
     </row>
     <row r="126" spans="1:16" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A126" s="75" t="s">
+      <c r="A126" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="B126" s="76"/>
-      <c r="C126" s="76"/>
-      <c r="D126" s="76"/>
-      <c r="E126" s="76"/>
-      <c r="F126" s="76"/>
-      <c r="G126" s="76"/>
-      <c r="H126" s="76"/>
-      <c r="I126" s="76"/>
-      <c r="J126" s="76"/>
-      <c r="K126" s="76"/>
-      <c r="L126" s="76"/>
-      <c r="M126" s="76"/>
-      <c r="N126" s="76"/>
+      <c r="B126" s="74"/>
+      <c r="C126" s="74"/>
+      <c r="D126" s="74"/>
+      <c r="E126" s="74"/>
+      <c r="F126" s="74"/>
+      <c r="G126" s="74"/>
+      <c r="H126" s="74"/>
+      <c r="I126" s="74"/>
+      <c r="J126" s="74"/>
+      <c r="K126" s="74"/>
+      <c r="L126" s="74"/>
+      <c r="M126" s="74"/>
+      <c r="N126" s="74"/>
     </row>
     <row r="127" spans="1:16" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A127" s="75" t="s">
+      <c r="A127" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="B127" s="76"/>
-      <c r="C127" s="76"/>
-      <c r="D127" s="76"/>
-      <c r="E127" s="76"/>
-      <c r="F127" s="76"/>
-      <c r="G127" s="76"/>
-      <c r="H127" s="76"/>
-      <c r="I127" s="76"/>
-      <c r="J127" s="76"/>
-      <c r="K127" s="76"/>
-      <c r="L127" s="76"/>
-      <c r="M127" s="76"/>
-      <c r="N127" s="76"/>
+      <c r="B127" s="74"/>
+      <c r="C127" s="74"/>
+      <c r="D127" s="74"/>
+      <c r="E127" s="74"/>
+      <c r="F127" s="74"/>
+      <c r="G127" s="74"/>
+      <c r="H127" s="74"/>
+      <c r="I127" s="74"/>
+      <c r="J127" s="74"/>
+      <c r="K127" s="74"/>
+      <c r="L127" s="74"/>
+      <c r="M127" s="74"/>
+      <c r="N127" s="74"/>
     </row>
     <row r="128" spans="1:16" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A128" s="75" t="s">
+      <c r="A128" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="B128" s="76"/>
-      <c r="C128" s="76"/>
-      <c r="D128" s="76"/>
-      <c r="E128" s="76"/>
-      <c r="F128" s="76"/>
-      <c r="G128" s="76"/>
-      <c r="H128" s="76"/>
-      <c r="I128" s="76"/>
-      <c r="J128" s="76"/>
-      <c r="K128" s="76"/>
-      <c r="L128" s="76"/>
-      <c r="M128" s="76"/>
-      <c r="N128" s="76"/>
+      <c r="B128" s="74"/>
+      <c r="C128" s="74"/>
+      <c r="D128" s="74"/>
+      <c r="E128" s="74"/>
+      <c r="F128" s="74"/>
+      <c r="G128" s="74"/>
+      <c r="H128" s="74"/>
+      <c r="I128" s="74"/>
+      <c r="J128" s="74"/>
+      <c r="K128" s="74"/>
+      <c r="L128" s="74"/>
+      <c r="M128" s="74"/>
+      <c r="N128" s="74"/>
     </row>
     <row r="129" spans="1:14" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A129" s="75" t="s">
+      <c r="A129" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="B129" s="76"/>
-      <c r="C129" s="76"/>
-      <c r="D129" s="76"/>
-      <c r="E129" s="76"/>
-      <c r="F129" s="76"/>
-      <c r="G129" s="76"/>
-      <c r="H129" s="76"/>
-      <c r="I129" s="76"/>
-      <c r="J129" s="76"/>
-      <c r="K129" s="76"/>
-      <c r="L129" s="76"/>
-      <c r="M129" s="76"/>
-      <c r="N129" s="76"/>
+      <c r="B129" s="74"/>
+      <c r="C129" s="74"/>
+      <c r="D129" s="74"/>
+      <c r="E129" s="74"/>
+      <c r="F129" s="74"/>
+      <c r="G129" s="74"/>
+      <c r="H129" s="74"/>
+      <c r="I129" s="74"/>
+      <c r="J129" s="74"/>
+      <c r="K129" s="74"/>
+      <c r="L129" s="74"/>
+      <c r="M129" s="74"/>
+      <c r="N129" s="74"/>
     </row>
     <row r="130" spans="1:14" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A130" s="75" t="s">
+      <c r="A130" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="B130" s="76"/>
-      <c r="C130" s="76"/>
-      <c r="D130" s="76"/>
-      <c r="E130" s="76"/>
-      <c r="F130" s="76"/>
-      <c r="G130" s="76"/>
-      <c r="H130" s="76"/>
-      <c r="I130" s="76"/>
-      <c r="J130" s="76"/>
-      <c r="K130" s="76"/>
-      <c r="L130" s="76"/>
-      <c r="M130" s="76"/>
-      <c r="N130" s="76"/>
+      <c r="B130" s="74"/>
+      <c r="C130" s="74"/>
+      <c r="D130" s="74"/>
+      <c r="E130" s="74"/>
+      <c r="F130" s="74"/>
+      <c r="G130" s="74"/>
+      <c r="H130" s="74"/>
+      <c r="I130" s="74"/>
+      <c r="J130" s="74"/>
+      <c r="K130" s="74"/>
+      <c r="L130" s="74"/>
+      <c r="M130" s="74"/>
+      <c r="N130" s="74"/>
     </row>
     <row r="131" spans="1:14" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A131" s="75" t="s">
+      <c r="A131" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="B131" s="76"/>
-      <c r="C131" s="76"/>
-      <c r="D131" s="76"/>
-      <c r="E131" s="76"/>
-      <c r="F131" s="76"/>
-      <c r="G131" s="76"/>
-      <c r="H131" s="76"/>
-      <c r="I131" s="76"/>
-      <c r="J131" s="76"/>
-      <c r="K131" s="76"/>
-      <c r="L131" s="76"/>
-      <c r="M131" s="76"/>
-      <c r="N131" s="76"/>
+      <c r="B131" s="74"/>
+      <c r="C131" s="74"/>
+      <c r="D131" s="74"/>
+      <c r="E131" s="74"/>
+      <c r="F131" s="74"/>
+      <c r="G131" s="74"/>
+      <c r="H131" s="74"/>
+      <c r="I131" s="74"/>
+      <c r="J131" s="74"/>
+      <c r="K131" s="74"/>
+      <c r="L131" s="74"/>
+      <c r="M131" s="74"/>
+      <c r="N131" s="74"/>
     </row>
     <row r="132" spans="1:14" s="69" customFormat="1" ht="9" x14ac:dyDescent="0.2">
-      <c r="A132" s="75" t="s">
+      <c r="A132" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="B132" s="76"/>
-      <c r="C132" s="76"/>
-      <c r="D132" s="76"/>
-      <c r="E132" s="76"/>
-      <c r="F132" s="76"/>
-      <c r="G132" s="76"/>
-      <c r="H132" s="76"/>
-      <c r="I132" s="76"/>
-      <c r="J132" s="76"/>
-      <c r="K132" s="76"/>
-      <c r="L132" s="76"/>
-      <c r="M132" s="76"/>
-      <c r="N132" s="76"/>
+      <c r="B132" s="74"/>
+      <c r="C132" s="74"/>
+      <c r="D132" s="74"/>
+      <c r="E132" s="74"/>
+      <c r="F132" s="74"/>
+      <c r="G132" s="74"/>
+      <c r="H132" s="74"/>
+      <c r="I132" s="74"/>
+      <c r="J132" s="74"/>
+      <c r="K132" s="74"/>
+      <c r="L132" s="74"/>
+      <c r="M132" s="74"/>
+      <c r="N132" s="74"/>
     </row>
     <row r="133" spans="1:14" s="69" customFormat="1" ht="9.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="73" t="s">
+      <c r="A133" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="B133" s="74"/>
-      <c r="C133" s="74"/>
-      <c r="D133" s="74"/>
-      <c r="E133" s="74"/>
-      <c r="F133" s="74"/>
-      <c r="G133" s="74"/>
-      <c r="H133" s="74"/>
-      <c r="I133" s="74"/>
-      <c r="J133" s="74"/>
-      <c r="K133" s="74"/>
-      <c r="L133" s="74"/>
-      <c r="M133" s="74"/>
-      <c r="N133" s="74"/>
+      <c r="B133" s="78"/>
+      <c r="C133" s="78"/>
+      <c r="D133" s="78"/>
+      <c r="E133" s="78"/>
+      <c r="F133" s="78"/>
+      <c r="G133" s="78"/>
+      <c r="H133" s="78"/>
+      <c r="I133" s="78"/>
+      <c r="J133" s="78"/>
+      <c r="K133" s="78"/>
+      <c r="L133" s="78"/>
+      <c r="M133" s="78"/>
+      <c r="N133" s="78"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="70" t="s">
@@ -7637,12 +7637,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A126:N126"/>
-    <mergeCell ref="A121:N121"/>
-    <mergeCell ref="A122:N122"/>
-    <mergeCell ref="A123:N123"/>
-    <mergeCell ref="A124:N124"/>
-    <mergeCell ref="A125:N125"/>
     <mergeCell ref="A133:N133"/>
     <mergeCell ref="A127:N127"/>
     <mergeCell ref="A128:N128"/>
@@ -7650,6 +7644,12 @@
     <mergeCell ref="A130:N130"/>
     <mergeCell ref="A131:N131"/>
     <mergeCell ref="A132:N132"/>
+    <mergeCell ref="A126:N126"/>
+    <mergeCell ref="A121:N121"/>
+    <mergeCell ref="A122:N122"/>
+    <mergeCell ref="A123:N123"/>
+    <mergeCell ref="A124:N124"/>
+    <mergeCell ref="A125:N125"/>
   </mergeCells>
   <printOptions gridLinesSet="0"/>
   <pageMargins left="0.47244094488188981" right="0.27559055118110237" top="0.18" bottom="0.16" header="0.19" footer="0.11811023622047245"/>
@@ -7677,7 +7677,9 @@
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7787,7 +7789,8 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>Data!B7</f>
+        <v>-5.4736901629041781E-2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -7893,7 +7896,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>